<commit_message>
Modificata la generazione del Conveyor_ID
</commit_message>
<xml_diff>
--- a/Input/IO_LIST/NT23_IO LIST API002_r3.xlsx
+++ b/Input/IO_LIST/NT23_IO LIST API002_r3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76BA527-3453-463B-922B-9B177647B641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F8E6D7-65B6-4113-82E3-6D5A3F824183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -2050,7 +2050,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3001,7 +3001,27 @@
     <cellStyle name="Normale 7 2" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
     <cellStyle name="Percent 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3345,13 +3365,13 @@
       <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="5" width="20.5703125" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="16"/>
+    <col min="1" max="5" width="20.59765625" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="8.73046875" style="16"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="13.15">
       <c r="A13" s="41" t="s">
         <v>342</v>
       </c>
@@ -3360,7 +3380,7 @@
       <c r="D13" s="42"/>
       <c r="E13" s="42"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="13.15">
       <c r="A14" s="28" t="s">
         <v>341</v>
       </c>
@@ -3377,7 +3397,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="14.45" customHeight="1">
       <c r="A15" s="25">
         <v>0</v>
       </c>
@@ -3392,7 +3412,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="25">
         <v>1</v>
       </c>
@@ -3407,7 +3427,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="14.25">
       <c r="A17" s="25">
         <v>2</v>
       </c>
@@ -3422,7 +3442,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="14.25">
       <c r="A18" s="25">
         <v>3</v>
       </c>
@@ -3437,28 +3457,28 @@
         <v>664</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="26"/>
       <c r="B19" s="24"/>
       <c r="C19" s="23"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="22"/>
       <c r="B20" s="24"/>
       <c r="C20" s="23"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="14.25">
       <c r="A21" s="25"/>
       <c r="B21" s="24"/>
       <c r="C21" s="23"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="14.25">
       <c r="A22" s="25"/>
       <c r="B22" s="24"/>
       <c r="C22" s="23"/>
@@ -3482,39 +3502,39 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.73046875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.73046875" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.3984375" style="16" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.1328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.1328125" style="16" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.7109375" style="16"/>
+    <col min="29" max="16384" width="8.73046875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="14.25">
       <c r="A1" s="43" t="s">
         <v>334</v>
       </c>
@@ -3548,7 +3568,7 @@
       <c r="AA1" s="43"/>
       <c r="AB1" s="43"/>
     </row>
-    <row r="2" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="14.25">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
@@ -3634,7 +3654,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="15.6" customHeight="1">
       <c r="A3" s="44" t="s">
         <v>345</v>
       </c>
@@ -3666,7 +3686,7 @@
       <c r="AA3" s="45"/>
       <c r="AB3" s="46"/>
     </row>
-    <row r="4" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="15">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="19" t="s">
@@ -3702,7 +3722,7 @@
       <c r="AA4" s="17"/>
       <c r="AB4" s="17"/>
     </row>
-    <row r="5" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="15">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="19" t="s">
@@ -3738,7 +3758,7 @@
       <c r="AA5" s="17"/>
       <c r="AB5" s="17"/>
     </row>
-    <row r="6" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="15">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="19" t="s">
@@ -3774,7 +3794,7 @@
       <c r="AA6" s="17"/>
       <c r="AB6" s="17"/>
     </row>
-    <row r="7" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="15">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="19" t="s">
@@ -3810,7 +3830,7 @@
       <c r="AA7" s="17"/>
       <c r="AB7" s="17"/>
     </row>
-    <row r="8" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="15">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="19" t="s">
@@ -3846,7 +3866,7 @@
       <c r="AA8" s="17"/>
       <c r="AB8" s="17"/>
     </row>
-    <row r="9" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="15">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="19" t="s">
@@ -3882,7 +3902,7 @@
       <c r="AA9" s="17"/>
       <c r="AB9" s="17"/>
     </row>
-    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="15">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
@@ -3918,7 +3938,7 @@
       <c r="AA10" s="17"/>
       <c r="AB10" s="17"/>
     </row>
-    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="15">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="19" t="s">
@@ -3954,7 +3974,7 @@
       <c r="AA11" s="17"/>
       <c r="AB11" s="17"/>
     </row>
-    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
@@ -3990,7 +4010,7 @@
       <c r="AA12" s="17"/>
       <c r="AB12" s="17"/>
     </row>
-    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
@@ -4026,7 +4046,7 @@
       <c r="AA13" s="17"/>
       <c r="AB13" s="17"/>
     </row>
-    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="19" t="s">
@@ -4062,7 +4082,7 @@
       <c r="AA14" s="17"/>
       <c r="AB14" s="17"/>
     </row>
-    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="15">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
@@ -4098,7 +4118,7 @@
       <c r="AA15" s="17"/>
       <c r="AB15" s="17"/>
     </row>
-    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="15">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
@@ -4134,7 +4154,7 @@
       <c r="AA16" s="17"/>
       <c r="AB16" s="17"/>
     </row>
-    <row r="17" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="15">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="19" t="s">
@@ -4170,7 +4190,7 @@
       <c r="AA17" s="17"/>
       <c r="AB17" s="17"/>
     </row>
-    <row r="18" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="15">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="19" t="s">
@@ -4206,7 +4226,7 @@
       <c r="AA18" s="17"/>
       <c r="AB18" s="17"/>
     </row>
-    <row r="19" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="15">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="19" t="s">
@@ -4242,7 +4262,7 @@
       <c r="AA19" s="17"/>
       <c r="AB19" s="17"/>
     </row>
-    <row r="20" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="15">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="19" t="s">
@@ -4278,7 +4298,7 @@
       <c r="AA20" s="17"/>
       <c r="AB20" s="17"/>
     </row>
-    <row r="21" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="15">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="19" t="s">
@@ -4314,7 +4334,7 @@
       <c r="AA21" s="17"/>
       <c r="AB21" s="17"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28">
       <c r="A22" s="44" t="s">
         <v>424</v>
       </c>
@@ -4346,7 +4366,7 @@
       <c r="AA22" s="45"/>
       <c r="AB22" s="46"/>
     </row>
-    <row r="23" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="15">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="19" t="s">
@@ -4380,7 +4400,7 @@
       <c r="AA23" s="17"/>
       <c r="AB23" s="17"/>
     </row>
-    <row r="24" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="15">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="19" t="s">
@@ -4414,7 +4434,7 @@
       <c r="AA24" s="17"/>
       <c r="AB24" s="17"/>
     </row>
-    <row r="25" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="15">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="19" t="s">
@@ -4448,7 +4468,7 @@
       <c r="AA25" s="17"/>
       <c r="AB25" s="17"/>
     </row>
-    <row r="26" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="15">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="19" t="s">
@@ -4499,30 +4519,30 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:V215"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="1" sqref="A173:XFD173 A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="87.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="93.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="17" width="8.59765625" customWidth="1"/>
+    <col min="18" max="18" width="10.3984375" customWidth="1"/>
+    <col min="19" max="19" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="50" t="s">
         <v>2</v>
       </c>
@@ -4554,7 +4574,7 @@
       <c r="U1" s="12"/>
       <c r="V1" s="12"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="56" t="s">
         <v>7</v>
       </c>
@@ -4586,7 +4606,7 @@
       </c>
       <c r="V2" s="9"/>
     </row>
-    <row r="3" spans="1:22" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="90.75">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -4654,7 +4674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
@@ -4717,7 +4737,7 @@
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
     </row>
-    <row r="5" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="14.45" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
@@ -4782,7 +4802,7 @@
       <c r="U5" s="14"/>
       <c r="V5" s="14"/>
     </row>
-    <row r="6" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="14.45" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>27</v>
       </c>
@@ -4847,7 +4867,7 @@
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
     </row>
-    <row r="7" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="14.45" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>27</v>
       </c>
@@ -4912,7 +4932,7 @@
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
     </row>
-    <row r="8" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="14.45" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>27</v>
       </c>
@@ -4975,7 +4995,7 @@
       <c r="U8" s="14"/>
       <c r="V8" s="14"/>
     </row>
-    <row r="9" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="14.45" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
@@ -5040,7 +5060,7 @@
       <c r="U9" s="14"/>
       <c r="V9" s="14"/>
     </row>
-    <row r="10" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="14.45" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>27</v>
       </c>
@@ -5105,7 +5125,7 @@
       <c r="U10" s="14"/>
       <c r="V10" s="14"/>
     </row>
-    <row r="11" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="14.45" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
@@ -5170,7 +5190,7 @@
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
     </row>
-    <row r="12" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="14.45" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>27</v>
       </c>
@@ -5235,7 +5255,7 @@
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
     </row>
-    <row r="13" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="14.45" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>429</v>
       </c>
@@ -5300,7 +5320,7 @@
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
     </row>
-    <row r="14" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="14.45" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>460</v>
       </c>
@@ -5361,7 +5381,7 @@
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
     </row>
-    <row r="15" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="14.45" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>429</v>
       </c>
@@ -5424,7 +5444,7 @@
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
     </row>
-    <row r="16" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="14.45" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>27</v>
       </c>
@@ -5489,7 +5509,7 @@
       <c r="U16" s="14"/>
       <c r="V16" s="14"/>
     </row>
-    <row r="17" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="14.45" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>429</v>
       </c>
@@ -5554,7 +5574,7 @@
       <c r="U17" s="14"/>
       <c r="V17" s="14"/>
     </row>
-    <row r="18" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="14.45" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>429</v>
       </c>
@@ -5617,7 +5637,7 @@
       <c r="U18" s="14"/>
       <c r="V18" s="14"/>
     </row>
-    <row r="19" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="14.45" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>429</v>
       </c>
@@ -5680,7 +5700,7 @@
       <c r="U19" s="14"/>
       <c r="V19" s="14"/>
     </row>
-    <row r="20" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="14.45" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>429</v>
       </c>
@@ -5729,7 +5749,7 @@
       <c r="U20" s="14"/>
       <c r="V20" s="14"/>
     </row>
-    <row r="21" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="14.45" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>429</v>
       </c>
@@ -5778,7 +5798,7 @@
       <c r="U21" s="14"/>
       <c r="V21" s="14"/>
     </row>
-    <row r="22" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="14.45" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>429</v>
       </c>
@@ -5825,7 +5845,7 @@
       <c r="U22" s="14"/>
       <c r="V22" s="14"/>
     </row>
-    <row r="23" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="14.45" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>429</v>
       </c>
@@ -5872,7 +5892,7 @@
       <c r="U23" s="14"/>
       <c r="V23" s="14"/>
     </row>
-    <row r="24" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="14.45" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>429</v>
       </c>
@@ -5919,7 +5939,7 @@
       <c r="U24" s="14"/>
       <c r="V24" s="14"/>
     </row>
-    <row r="25" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="14.45" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>429</v>
       </c>
@@ -5966,7 +5986,7 @@
       <c r="U25" s="14"/>
       <c r="V25" s="14"/>
     </row>
-    <row r="26" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="14.45" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>429</v>
       </c>
@@ -6013,7 +6033,7 @@
       <c r="U26" s="14"/>
       <c r="V26" s="14"/>
     </row>
-    <row r="27" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="14.45" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>429</v>
       </c>
@@ -6029,7 +6049,7 @@
         <v>442</v>
       </c>
       <c r="G27" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(IF(LEFT(F27,1)="=",RIGHT(F27,LEN(F27)-1),F27)&amp;"_"&amp;H27," - ","_"),"-","_")," ","_"),"+","_"),":","_"),".","_"),"NT23__",""),"__","_"),"__","_"),"__","_"),"__","_"),"AE00_",""),"AE01_",""),"&amp;_",""),",",""),"/","")</f>
         <v>MCPHF11_400X1_11_SPARE</v>
       </c>
       <c r="H27" s="14" t="s">
@@ -6060,7 +6080,7 @@
       <c r="U27" s="14"/>
       <c r="V27" s="14"/>
     </row>
-    <row r="28" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="14.45" customHeight="1">
       <c r="A28" s="14" t="s">
         <v>429</v>
       </c>
@@ -6123,7 +6143,7 @@
       <c r="U28" s="14"/>
       <c r="V28" s="14"/>
     </row>
-    <row r="29" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="14.45" customHeight="1">
       <c r="A29" s="14" t="s">
         <v>429</v>
       </c>
@@ -6186,7 +6206,7 @@
       <c r="U29" s="14"/>
       <c r="V29" s="14"/>
     </row>
-    <row r="30" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="14.45" customHeight="1">
       <c r="A30" s="14" t="s">
         <v>429</v>
       </c>
@@ -6249,7 +6269,7 @@
       <c r="U30" s="14"/>
       <c r="V30" s="14"/>
     </row>
-    <row r="31" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="14.45" customHeight="1">
       <c r="A31" s="14" t="s">
         <v>429</v>
       </c>
@@ -6312,7 +6332,7 @@
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
     </row>
-    <row r="32" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="14.45" customHeight="1">
       <c r="A32" s="14" t="s">
         <v>429</v>
       </c>
@@ -6375,7 +6395,7 @@
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
     </row>
-    <row r="33" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="14.45" customHeight="1">
       <c r="A33" s="14" t="s">
         <v>429</v>
       </c>
@@ -6438,7 +6458,7 @@
       <c r="U33" s="14"/>
       <c r="V33" s="14"/>
     </row>
-    <row r="34" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="14.45" customHeight="1">
       <c r="A34" s="14" t="s">
         <v>429</v>
       </c>
@@ -6501,7 +6521,7 @@
       <c r="U34" s="14"/>
       <c r="V34" s="14"/>
     </row>
-    <row r="35" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="14.45" customHeight="1">
       <c r="A35" s="14" t="s">
         <v>429</v>
       </c>
@@ -6564,7 +6584,7 @@
       <c r="U35" s="14"/>
       <c r="V35" s="14"/>
     </row>
-    <row r="36" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="14.45" customHeight="1">
       <c r="A36" s="14" t="s">
         <v>429</v>
       </c>
@@ -6627,7 +6647,7 @@
       <c r="U36" s="14"/>
       <c r="V36" s="14"/>
     </row>
-    <row r="37" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="14.45" customHeight="1">
       <c r="A37" s="14" t="s">
         <v>429</v>
       </c>
@@ -6690,7 +6710,7 @@
       <c r="U37" s="14"/>
       <c r="V37" s="14"/>
     </row>
-    <row r="38" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="14.45" customHeight="1">
       <c r="A38" s="14" t="s">
         <v>429</v>
       </c>
@@ -6753,7 +6773,7 @@
       <c r="U38" s="14"/>
       <c r="V38" s="14"/>
     </row>
-    <row r="39" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="14.45" customHeight="1">
       <c r="A39" s="14" t="s">
         <v>460</v>
       </c>
@@ -6816,7 +6836,7 @@
       <c r="U39" s="14"/>
       <c r="V39" s="14"/>
     </row>
-    <row r="40" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="14.45" customHeight="1">
       <c r="A40" s="14" t="s">
         <v>429</v>
       </c>
@@ -6879,7 +6899,7 @@
       <c r="U40" s="14"/>
       <c r="V40" s="14"/>
     </row>
-    <row r="41" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="14.45" customHeight="1">
       <c r="A41" s="14" t="s">
         <v>429</v>
       </c>
@@ -6942,7 +6962,7 @@
       <c r="U41" s="14"/>
       <c r="V41" s="14"/>
     </row>
-    <row r="42" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="14.45" customHeight="1">
       <c r="A42" s="14" t="s">
         <v>429</v>
       </c>
@@ -7005,7 +7025,7 @@
       <c r="U42" s="14"/>
       <c r="V42" s="14"/>
     </row>
-    <row r="43" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="14.45" customHeight="1">
       <c r="A43" s="14" t="s">
         <v>429</v>
       </c>
@@ -7068,7 +7088,7 @@
       <c r="U43" s="14"/>
       <c r="V43" s="14"/>
     </row>
-    <row r="44" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="14.45" customHeight="1">
       <c r="A44" s="14" t="s">
         <v>429</v>
       </c>
@@ -7131,7 +7151,7 @@
       <c r="U44" s="14"/>
       <c r="V44" s="14"/>
     </row>
-    <row r="45" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="14.45" customHeight="1">
       <c r="A45" s="14" t="s">
         <v>429</v>
       </c>
@@ -7194,7 +7214,7 @@
       <c r="U45" s="14"/>
       <c r="V45" s="14"/>
     </row>
-    <row r="46" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="14.45" customHeight="1">
       <c r="A46" s="14" t="s">
         <v>429</v>
       </c>
@@ -7257,7 +7277,7 @@
       <c r="U46" s="14"/>
       <c r="V46" s="14"/>
     </row>
-    <row r="47" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="14.45" customHeight="1">
       <c r="A47" s="14" t="s">
         <v>429</v>
       </c>
@@ -7320,7 +7340,7 @@
       <c r="U47" s="14"/>
       <c r="V47" s="14"/>
     </row>
-    <row r="48" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="14.45" customHeight="1">
       <c r="A48" s="14" t="s">
         <v>429</v>
       </c>
@@ -7383,7 +7403,7 @@
       <c r="U48" s="14"/>
       <c r="V48" s="14"/>
     </row>
-    <row r="49" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="14.45" customHeight="1">
       <c r="A49" s="14" t="s">
         <v>429</v>
       </c>
@@ -7446,7 +7466,7 @@
       <c r="U49" s="14"/>
       <c r="V49" s="14"/>
     </row>
-    <row r="50" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="14.45" customHeight="1">
       <c r="A50" s="14" t="s">
         <v>429</v>
       </c>
@@ -7509,7 +7529,7 @@
       <c r="U50" s="14"/>
       <c r="V50" s="14"/>
     </row>
-    <row r="51" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="14.45" customHeight="1">
       <c r="A51" s="14" t="s">
         <v>429</v>
       </c>
@@ -7572,7 +7592,7 @@
       <c r="U51" s="14"/>
       <c r="V51" s="14"/>
     </row>
-    <row r="52" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" ht="14.45" customHeight="1">
       <c r="A52" s="14" t="s">
         <v>429</v>
       </c>
@@ -7635,7 +7655,7 @@
       <c r="U52" s="14"/>
       <c r="V52" s="14"/>
     </row>
-    <row r="53" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" ht="14.45" customHeight="1">
       <c r="A53" s="14" t="s">
         <v>429</v>
       </c>
@@ -7698,7 +7718,7 @@
       <c r="U53" s="14"/>
       <c r="V53" s="14"/>
     </row>
-    <row r="54" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" ht="14.45" customHeight="1">
       <c r="A54" s="14" t="s">
         <v>429</v>
       </c>
@@ -7761,7 +7781,7 @@
       <c r="U54" s="14"/>
       <c r="V54" s="14"/>
     </row>
-    <row r="55" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" ht="14.45" customHeight="1">
       <c r="A55" s="14" t="s">
         <v>460</v>
       </c>
@@ -7826,7 +7846,7 @@
       <c r="U55" s="14"/>
       <c r="V55" s="14"/>
     </row>
-    <row r="56" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="14.45" customHeight="1">
       <c r="A56" s="14" t="s">
         <v>460</v>
       </c>
@@ -7889,7 +7909,7 @@
       <c r="U56" s="14"/>
       <c r="V56" s="14"/>
     </row>
-    <row r="57" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="14.45" customHeight="1">
       <c r="A57" s="14" t="s">
         <v>460</v>
       </c>
@@ -7954,7 +7974,7 @@
       <c r="U57" s="14"/>
       <c r="V57" s="14"/>
     </row>
-    <row r="58" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="14.45" customHeight="1">
       <c r="A58" s="14" t="s">
         <v>460</v>
       </c>
@@ -8017,7 +8037,7 @@
       <c r="U58" s="14"/>
       <c r="V58" s="14"/>
     </row>
-    <row r="59" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="14.45" customHeight="1">
       <c r="A59" s="14" t="s">
         <v>429</v>
       </c>
@@ -8080,7 +8100,7 @@
       <c r="U59" s="14"/>
       <c r="V59" s="14"/>
     </row>
-    <row r="60" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="14.45" customHeight="1">
       <c r="A60" s="14" t="s">
         <v>460</v>
       </c>
@@ -8145,7 +8165,7 @@
       <c r="U60" s="14"/>
       <c r="V60" s="14"/>
     </row>
-    <row r="61" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="14.45" customHeight="1">
       <c r="A61" s="14" t="s">
         <v>460</v>
       </c>
@@ -8208,7 +8228,7 @@
       <c r="U61" s="14"/>
       <c r="V61" s="14"/>
     </row>
-    <row r="62" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="14.45" customHeight="1">
       <c r="A62" s="14" t="s">
         <v>460</v>
       </c>
@@ -8273,7 +8293,7 @@
       <c r="U62" s="14"/>
       <c r="V62" s="14"/>
     </row>
-    <row r="63" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="14.45" customHeight="1">
       <c r="A63" s="14" t="s">
         <v>460</v>
       </c>
@@ -8336,7 +8356,7 @@
       <c r="U63" s="14"/>
       <c r="V63" s="14"/>
     </row>
-    <row r="64" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="14.45" customHeight="1">
       <c r="A64" s="14" t="s">
         <v>429</v>
       </c>
@@ -8401,7 +8421,7 @@
       <c r="U64" s="14"/>
       <c r="V64" s="14"/>
     </row>
-    <row r="65" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" ht="14.45" customHeight="1">
       <c r="A65" s="14" t="s">
         <v>429</v>
       </c>
@@ -8466,7 +8486,7 @@
       <c r="U65" s="14"/>
       <c r="V65" s="14"/>
     </row>
-    <row r="66" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" ht="14.45" customHeight="1">
       <c r="A66" s="14" t="s">
         <v>429</v>
       </c>
@@ -8531,7 +8551,7 @@
       <c r="U66" s="14"/>
       <c r="V66" s="14"/>
     </row>
-    <row r="67" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" ht="14.45" customHeight="1">
       <c r="A67" s="14" t="s">
         <v>429</v>
       </c>
@@ -8596,7 +8616,7 @@
       <c r="U67" s="14"/>
       <c r="V67" s="14"/>
     </row>
-    <row r="68" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" ht="14.45" customHeight="1">
       <c r="A68" s="14" t="s">
         <v>429</v>
       </c>
@@ -8661,7 +8681,7 @@
       <c r="U68" s="14"/>
       <c r="V68" s="14"/>
     </row>
-    <row r="69" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" ht="14.45" customHeight="1">
       <c r="A69" s="14" t="s">
         <v>429</v>
       </c>
@@ -8726,7 +8746,7 @@
       <c r="U69" s="14"/>
       <c r="V69" s="14"/>
     </row>
-    <row r="70" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" ht="14.45" customHeight="1">
       <c r="A70" s="14" t="s">
         <v>429</v>
       </c>
@@ -8791,7 +8811,7 @@
       <c r="U70" s="14"/>
       <c r="V70" s="14"/>
     </row>
-    <row r="71" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" ht="14.45" customHeight="1">
       <c r="A71" s="14" t="s">
         <v>429</v>
       </c>
@@ -8856,7 +8876,7 @@
       <c r="U71" s="14"/>
       <c r="V71" s="14"/>
     </row>
-    <row r="72" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" ht="14.45" customHeight="1">
       <c r="A72" s="14" t="s">
         <v>429</v>
       </c>
@@ -8921,7 +8941,7 @@
       <c r="U72" s="14"/>
       <c r="V72" s="14"/>
     </row>
-    <row r="73" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" ht="14.45" customHeight="1">
       <c r="A73" s="14" t="s">
         <v>429</v>
       </c>
@@ -8986,7 +9006,7 @@
       <c r="U73" s="14"/>
       <c r="V73" s="14"/>
     </row>
-    <row r="74" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" ht="14.45" customHeight="1">
       <c r="A74" s="14" t="s">
         <v>429</v>
       </c>
@@ -9051,7 +9071,7 @@
       <c r="U74" s="14"/>
       <c r="V74" s="14"/>
     </row>
-    <row r="75" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" ht="14.45" customHeight="1">
       <c r="A75" s="14" t="s">
         <v>429</v>
       </c>
@@ -9116,7 +9136,7 @@
       <c r="U75" s="14"/>
       <c r="V75" s="14"/>
     </row>
-    <row r="76" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" ht="14.45" customHeight="1">
       <c r="A76" s="14" t="s">
         <v>429</v>
       </c>
@@ -9181,7 +9201,7 @@
       <c r="U76" s="14"/>
       <c r="V76" s="14"/>
     </row>
-    <row r="77" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" ht="14.45" customHeight="1">
       <c r="A77" s="14" t="s">
         <v>429</v>
       </c>
@@ -9246,7 +9266,7 @@
       <c r="U77" s="14"/>
       <c r="V77" s="14"/>
     </row>
-    <row r="78" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" ht="14.45" customHeight="1">
       <c r="A78" s="14" t="s">
         <v>429</v>
       </c>
@@ -9311,7 +9331,7 @@
       <c r="U78" s="14"/>
       <c r="V78" s="14"/>
     </row>
-    <row r="79" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" ht="14.45" customHeight="1">
       <c r="A79" s="14" t="s">
         <v>429</v>
       </c>
@@ -9376,7 +9396,7 @@
       <c r="U79" s="14"/>
       <c r="V79" s="14"/>
     </row>
-    <row r="80" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" ht="14.45" customHeight="1">
       <c r="A80" s="14" t="s">
         <v>429</v>
       </c>
@@ -9441,7 +9461,7 @@
       <c r="U80" s="14"/>
       <c r="V80" s="14"/>
     </row>
-    <row r="81" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" ht="14.45" customHeight="1">
       <c r="A81" s="14" t="s">
         <v>429</v>
       </c>
@@ -9506,7 +9526,7 @@
       <c r="U81" s="14"/>
       <c r="V81" s="14"/>
     </row>
-    <row r="82" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" ht="14.45" customHeight="1">
       <c r="A82" s="14" t="s">
         <v>460</v>
       </c>
@@ -9569,7 +9589,7 @@
       <c r="U82" s="14"/>
       <c r="V82" s="14"/>
     </row>
-    <row r="83" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" ht="14.45" customHeight="1">
       <c r="A83" s="14" t="s">
         <v>460</v>
       </c>
@@ -9632,7 +9652,7 @@
       <c r="U83" s="14"/>
       <c r="V83" s="14"/>
     </row>
-    <row r="84" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" ht="14.45" customHeight="1">
       <c r="A84" s="14" t="s">
         <v>460</v>
       </c>
@@ -9695,7 +9715,7 @@
       <c r="U84" s="14"/>
       <c r="V84" s="14"/>
     </row>
-    <row r="85" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" ht="14.45" customHeight="1">
       <c r="A85" s="14" t="s">
         <v>460</v>
       </c>
@@ -9758,7 +9778,7 @@
       <c r="U85" s="14"/>
       <c r="V85" s="14"/>
     </row>
-    <row r="86" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" ht="14.45" customHeight="1">
       <c r="A86" s="14" t="s">
         <v>460</v>
       </c>
@@ -9821,7 +9841,7 @@
       <c r="U86" s="14"/>
       <c r="V86" s="14"/>
     </row>
-    <row r="87" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" ht="14.45" customHeight="1">
       <c r="A87" s="14" t="s">
         <v>460</v>
       </c>
@@ -9884,7 +9904,7 @@
       <c r="U87" s="14"/>
       <c r="V87" s="14"/>
     </row>
-    <row r="88" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" ht="14.45" customHeight="1">
       <c r="A88" s="14" t="s">
         <v>460</v>
       </c>
@@ -9947,7 +9967,7 @@
       <c r="U88" s="14"/>
       <c r="V88" s="14"/>
     </row>
-    <row r="89" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" ht="14.45" customHeight="1">
       <c r="A89" s="14" t="s">
         <v>460</v>
       </c>
@@ -10010,7 +10030,7 @@
       <c r="U89" s="14"/>
       <c r="V89" s="14"/>
     </row>
-    <row r="90" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" ht="14.45" customHeight="1">
       <c r="A90" s="14" t="s">
         <v>460</v>
       </c>
@@ -10073,7 +10093,7 @@
       <c r="U90" s="14"/>
       <c r="V90" s="14"/>
     </row>
-    <row r="91" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" ht="14.45" customHeight="1">
       <c r="A91" s="14" t="s">
         <v>460</v>
       </c>
@@ -10136,7 +10156,7 @@
       <c r="U91" s="14"/>
       <c r="V91" s="14"/>
     </row>
-    <row r="92" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" ht="14.45" customHeight="1">
       <c r="A92" s="14" t="s">
         <v>27</v>
       </c>
@@ -10197,7 +10217,7 @@
       <c r="U92" s="14"/>
       <c r="V92" s="14"/>
     </row>
-    <row r="93" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" ht="14.45" customHeight="1">
       <c r="A93" s="14" t="s">
         <v>27</v>
       </c>
@@ -10258,7 +10278,7 @@
       <c r="U93" s="14"/>
       <c r="V93" s="14"/>
     </row>
-    <row r="94" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" ht="14.45" customHeight="1">
       <c r="A94" s="14" t="s">
         <v>27</v>
       </c>
@@ -10319,7 +10339,7 @@
       <c r="U94" s="14"/>
       <c r="V94" s="14"/>
     </row>
-    <row r="95" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" ht="14.45" customHeight="1">
       <c r="A95" s="14" t="s">
         <v>460</v>
       </c>
@@ -10382,7 +10402,7 @@
       <c r="U95" s="14"/>
       <c r="V95" s="14"/>
     </row>
-    <row r="96" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" ht="14.45" customHeight="1">
       <c r="A96" s="14" t="s">
         <v>460</v>
       </c>
@@ -10447,7 +10467,7 @@
       <c r="U96" s="14"/>
       <c r="V96" s="14"/>
     </row>
-    <row r="97" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" ht="14.45" customHeight="1">
       <c r="A97" s="14" t="s">
         <v>460</v>
       </c>
@@ -10512,7 +10532,7 @@
       <c r="U97" s="14"/>
       <c r="V97" s="14"/>
     </row>
-    <row r="98" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" ht="14.45" customHeight="1">
       <c r="A98" s="14" t="s">
         <v>460</v>
       </c>
@@ -10577,7 +10597,7 @@
       <c r="U98" s="14"/>
       <c r="V98" s="14"/>
     </row>
-    <row r="99" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" ht="14.45" customHeight="1">
       <c r="A99" s="14" t="s">
         <v>27</v>
       </c>
@@ -10640,7 +10660,7 @@
       <c r="U99" s="14"/>
       <c r="V99" s="14"/>
     </row>
-    <row r="100" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" ht="14.45" customHeight="1">
       <c r="A100" s="14" t="s">
         <v>27</v>
       </c>
@@ -10703,7 +10723,7 @@
       <c r="U100" s="14"/>
       <c r="V100" s="14"/>
     </row>
-    <row r="101" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" ht="14.45" customHeight="1">
       <c r="A101" s="14" t="s">
         <v>27</v>
       </c>
@@ -10766,7 +10786,7 @@
       <c r="U101" s="14"/>
       <c r="V101" s="14"/>
     </row>
-    <row r="102" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" ht="14.45" customHeight="1">
       <c r="A102" s="14" t="s">
         <v>27</v>
       </c>
@@ -10829,7 +10849,7 @@
       <c r="U102" s="14"/>
       <c r="V102" s="14"/>
     </row>
-    <row r="103" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" ht="14.45" customHeight="1">
       <c r="A103" s="14" t="s">
         <v>27</v>
       </c>
@@ -10892,7 +10912,7 @@
       <c r="U103" s="14"/>
       <c r="V103" s="14"/>
     </row>
-    <row r="104" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" ht="14.45" customHeight="1">
       <c r="A104" s="14" t="s">
         <v>460</v>
       </c>
@@ -10957,7 +10977,7 @@
       <c r="U104" s="14"/>
       <c r="V104" s="14"/>
     </row>
-    <row r="105" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" ht="14.45" customHeight="1">
       <c r="A105" s="14" t="s">
         <v>460</v>
       </c>
@@ -11022,7 +11042,7 @@
       <c r="U105" s="14"/>
       <c r="V105" s="14"/>
     </row>
-    <row r="106" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" ht="14.45" customHeight="1">
       <c r="A106" s="14" t="s">
         <v>27</v>
       </c>
@@ -11087,7 +11107,7 @@
       <c r="U106" s="14"/>
       <c r="V106" s="14"/>
     </row>
-    <row r="107" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" ht="14.45" customHeight="1">
       <c r="A107" s="14" t="s">
         <v>27</v>
       </c>
@@ -11152,7 +11172,7 @@
       <c r="U107" s="14"/>
       <c r="V107" s="14"/>
     </row>
-    <row r="108" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" ht="14.45" customHeight="1">
       <c r="A108" s="14" t="s">
         <v>27</v>
       </c>
@@ -11217,7 +11237,7 @@
       <c r="U108" s="14"/>
       <c r="V108" s="14"/>
     </row>
-    <row r="109" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" ht="14.45" customHeight="1">
       <c r="A109" s="14" t="s">
         <v>27</v>
       </c>
@@ -11282,7 +11302,7 @@
       <c r="U109" s="14"/>
       <c r="V109" s="14"/>
     </row>
-    <row r="110" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" ht="14.45" customHeight="1">
       <c r="A110" s="14" t="s">
         <v>27</v>
       </c>
@@ -11347,7 +11367,7 @@
       <c r="U110" s="14"/>
       <c r="V110" s="14"/>
     </row>
-    <row r="111" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" ht="14.45" customHeight="1">
       <c r="A111" s="14" t="s">
         <v>27</v>
       </c>
@@ -11412,7 +11432,7 @@
       <c r="U111" s="14"/>
       <c r="V111" s="14"/>
     </row>
-    <row r="112" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" ht="14.45" customHeight="1">
       <c r="A112" s="14" t="s">
         <v>27</v>
       </c>
@@ -11477,7 +11497,7 @@
       <c r="U112" s="14"/>
       <c r="V112" s="14"/>
     </row>
-    <row r="113" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" ht="14.45" customHeight="1">
       <c r="A113" s="14" t="s">
         <v>27</v>
       </c>
@@ -11542,7 +11562,7 @@
       <c r="U113" s="14"/>
       <c r="V113" s="14"/>
     </row>
-    <row r="114" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" ht="14.45" customHeight="1">
       <c r="A114" s="14" t="s">
         <v>27</v>
       </c>
@@ -11607,7 +11627,7 @@
       <c r="U114" s="14"/>
       <c r="V114" s="14"/>
     </row>
-    <row r="115" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" ht="14.45" customHeight="1">
       <c r="A115" s="14" t="s">
         <v>27</v>
       </c>
@@ -11672,7 +11692,7 @@
       <c r="U115" s="14"/>
       <c r="V115" s="14"/>
     </row>
-    <row r="116" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" ht="14.45" customHeight="1">
       <c r="A116" s="14" t="s">
         <v>27</v>
       </c>
@@ -11737,7 +11757,7 @@
       <c r="U116" s="14"/>
       <c r="V116" s="14"/>
     </row>
-    <row r="117" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" ht="14.45" customHeight="1">
       <c r="A117" s="14" t="s">
         <v>27</v>
       </c>
@@ -11802,7 +11822,7 @@
       <c r="U117" s="14"/>
       <c r="V117" s="14"/>
     </row>
-    <row r="118" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" ht="14.45" customHeight="1">
       <c r="A118" s="14" t="s">
         <v>27</v>
       </c>
@@ -11867,7 +11887,7 @@
       <c r="U118" s="14"/>
       <c r="V118" s="14"/>
     </row>
-    <row r="119" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" ht="14.45" customHeight="1">
       <c r="A119" s="14" t="s">
         <v>27</v>
       </c>
@@ -11932,7 +11952,7 @@
       <c r="U119" s="14"/>
       <c r="V119" s="14"/>
     </row>
-    <row r="120" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" ht="14.45" customHeight="1">
       <c r="A120" s="14" t="s">
         <v>27</v>
       </c>
@@ -11997,7 +12017,7 @@
       <c r="U120" s="14"/>
       <c r="V120" s="14"/>
     </row>
-    <row r="121" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" ht="14.45" customHeight="1">
       <c r="A121" s="14" t="s">
         <v>27</v>
       </c>
@@ -12062,7 +12082,7 @@
       <c r="U121" s="14"/>
       <c r="V121" s="14"/>
     </row>
-    <row r="122" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" ht="14.45" customHeight="1">
       <c r="A122" s="14" t="s">
         <v>27</v>
       </c>
@@ -12127,7 +12147,7 @@
       <c r="U122" s="14"/>
       <c r="V122" s="14"/>
     </row>
-    <row r="123" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" ht="14.45" customHeight="1">
       <c r="A123" s="14" t="s">
         <v>27</v>
       </c>
@@ -12190,7 +12210,7 @@
       <c r="U123" s="14"/>
       <c r="V123" s="14"/>
     </row>
-    <row r="124" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" ht="14.45" customHeight="1">
       <c r="A124" s="14" t="s">
         <v>27</v>
       </c>
@@ -12255,7 +12275,7 @@
       <c r="U124" s="14"/>
       <c r="V124" s="14"/>
     </row>
-    <row r="125" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" ht="14.45" customHeight="1">
       <c r="A125" s="14" t="s">
         <v>27</v>
       </c>
@@ -12320,7 +12340,7 @@
       <c r="U125" s="14"/>
       <c r="V125" s="14"/>
     </row>
-    <row r="126" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" ht="14.45" customHeight="1">
       <c r="A126" s="14" t="s">
         <v>27</v>
       </c>
@@ -12385,7 +12405,7 @@
       <c r="U126" s="14"/>
       <c r="V126" s="14"/>
     </row>
-    <row r="127" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" ht="14.45" customHeight="1">
       <c r="A127" s="14" t="s">
         <v>27</v>
       </c>
@@ -12450,7 +12470,7 @@
       <c r="U127" s="14"/>
       <c r="V127" s="14"/>
     </row>
-    <row r="128" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" ht="14.45" customHeight="1">
       <c r="A128" s="14" t="s">
         <v>27</v>
       </c>
@@ -12515,7 +12535,7 @@
       <c r="U128" s="14"/>
       <c r="V128" s="14"/>
     </row>
-    <row r="129" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" ht="14.45" customHeight="1">
       <c r="A129" s="14" t="s">
         <v>27</v>
       </c>
@@ -12580,7 +12600,7 @@
       <c r="U129" s="14"/>
       <c r="V129" s="14"/>
     </row>
-    <row r="130" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" ht="14.45" customHeight="1">
       <c r="A130" s="14" t="s">
         <v>27</v>
       </c>
@@ -12645,7 +12665,7 @@
       <c r="U130" s="14"/>
       <c r="V130" s="14"/>
     </row>
-    <row r="131" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" ht="14.45" customHeight="1">
       <c r="A131" s="14" t="s">
         <v>27</v>
       </c>
@@ -12710,7 +12730,7 @@
       <c r="U131" s="14"/>
       <c r="V131" s="14"/>
     </row>
-    <row r="132" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" ht="14.45" customHeight="1">
       <c r="A132" s="14" t="s">
         <v>27</v>
       </c>
@@ -12773,7 +12793,7 @@
       <c r="U132" s="14"/>
       <c r="V132" s="14"/>
     </row>
-    <row r="133" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" ht="14.45" customHeight="1">
       <c r="A133" s="14" t="s">
         <v>27</v>
       </c>
@@ -12836,7 +12856,7 @@
       <c r="U133" s="14"/>
       <c r="V133" s="14"/>
     </row>
-    <row r="134" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" ht="14.45" customHeight="1">
       <c r="A134" s="14" t="s">
         <v>27</v>
       </c>
@@ -12899,7 +12919,7 @@
       <c r="U134" s="14"/>
       <c r="V134" s="14"/>
     </row>
-    <row r="135" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" ht="14.45" customHeight="1">
       <c r="A135" s="14" t="s">
         <v>27</v>
       </c>
@@ -12962,7 +12982,7 @@
       <c r="U135" s="14"/>
       <c r="V135" s="14"/>
     </row>
-    <row r="136" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" ht="14.45" customHeight="1">
       <c r="A136" s="14" t="s">
         <v>27</v>
       </c>
@@ -13025,7 +13045,7 @@
       <c r="U136" s="14"/>
       <c r="V136" s="14"/>
     </row>
-    <row r="137" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" ht="14.45" customHeight="1">
       <c r="A137" s="14" t="s">
         <v>27</v>
       </c>
@@ -13088,7 +13108,7 @@
       <c r="U137" s="14"/>
       <c r="V137" s="14"/>
     </row>
-    <row r="138" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" ht="14.45" customHeight="1">
       <c r="A138" s="14" t="s">
         <v>429</v>
       </c>
@@ -13153,7 +13173,7 @@
       <c r="U138" s="14"/>
       <c r="V138" s="14"/>
     </row>
-    <row r="139" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" ht="14.45" customHeight="1">
       <c r="A139" s="14" t="s">
         <v>429</v>
       </c>
@@ -13216,7 +13236,7 @@
       <c r="U139" s="14"/>
       <c r="V139" s="14"/>
     </row>
-    <row r="140" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" ht="14.45" customHeight="1">
       <c r="A140" s="14" t="s">
         <v>429</v>
       </c>
@@ -13279,7 +13299,7 @@
       <c r="U140" s="14"/>
       <c r="V140" s="14"/>
     </row>
-    <row r="141" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" ht="14.45" customHeight="1">
       <c r="A141" s="14" t="s">
         <v>429</v>
       </c>
@@ -13342,7 +13362,7 @@
       <c r="U141" s="14"/>
       <c r="V141" s="14"/>
     </row>
-    <row r="142" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" ht="14.45" customHeight="1">
       <c r="A142" s="14" t="s">
         <v>429</v>
       </c>
@@ -13405,7 +13425,7 @@
       <c r="U142" s="14"/>
       <c r="V142" s="14"/>
     </row>
-    <row r="143" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" ht="14.45" customHeight="1">
       <c r="A143" s="14" t="s">
         <v>429</v>
       </c>
@@ -13468,7 +13488,7 @@
       <c r="U143" s="14"/>
       <c r="V143" s="14"/>
     </row>
-    <row r="144" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" ht="14.45" customHeight="1">
       <c r="A144" s="14" t="s">
         <v>429</v>
       </c>
@@ -13531,7 +13551,7 @@
       <c r="U144" s="14"/>
       <c r="V144" s="14"/>
     </row>
-    <row r="145" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" ht="14.45" customHeight="1">
       <c r="A145" s="14" t="s">
         <v>429</v>
       </c>
@@ -13594,7 +13614,7 @@
       <c r="U145" s="14"/>
       <c r="V145" s="14"/>
     </row>
-    <row r="146" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" ht="14.45" customHeight="1">
       <c r="A146" s="14" t="s">
         <v>429</v>
       </c>
@@ -13657,7 +13677,7 @@
       <c r="U146" s="14"/>
       <c r="V146" s="14"/>
     </row>
-    <row r="147" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" ht="14.45" customHeight="1">
       <c r="A147" s="14" t="s">
         <v>429</v>
       </c>
@@ -13720,7 +13740,7 @@
       <c r="U147" s="14"/>
       <c r="V147" s="14"/>
     </row>
-    <row r="148" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" ht="14.45" customHeight="1">
       <c r="A148" s="14" t="s">
         <v>429</v>
       </c>
@@ -13783,7 +13803,7 @@
       <c r="U148" s="14"/>
       <c r="V148" s="14"/>
     </row>
-    <row r="149" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" ht="14.45" customHeight="1">
       <c r="A149" s="14" t="s">
         <v>429</v>
       </c>
@@ -13846,7 +13866,7 @@
       <c r="U149" s="14"/>
       <c r="V149" s="14"/>
     </row>
-    <row r="150" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" ht="14.45" customHeight="1">
       <c r="A150" s="14" t="s">
         <v>429</v>
       </c>
@@ -13909,7 +13929,7 @@
       <c r="U150" s="14"/>
       <c r="V150" s="14"/>
     </row>
-    <row r="151" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" ht="14.45" customHeight="1">
       <c r="A151" s="14" t="s">
         <v>429</v>
       </c>
@@ -13972,7 +13992,7 @@
       <c r="U151" s="14"/>
       <c r="V151" s="14"/>
     </row>
-    <row r="152" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" ht="14.45" customHeight="1">
       <c r="A152" s="14" t="s">
         <v>429</v>
       </c>
@@ -14035,7 +14055,7 @@
       <c r="U152" s="14"/>
       <c r="V152" s="14"/>
     </row>
-    <row r="153" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" ht="14.45" customHeight="1">
       <c r="A153" s="14" t="s">
         <v>429</v>
       </c>
@@ -14098,7 +14118,7 @@
       <c r="U153" s="14"/>
       <c r="V153" s="14"/>
     </row>
-    <row r="154" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" ht="14.45" customHeight="1">
       <c r="A154" s="14" t="s">
         <v>429</v>
       </c>
@@ -14161,7 +14181,7 @@
       <c r="U154" s="14"/>
       <c r="V154" s="14"/>
     </row>
-    <row r="155" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" ht="14.45" customHeight="1">
       <c r="A155" s="14" t="s">
         <v>429</v>
       </c>
@@ -14224,7 +14244,7 @@
       <c r="U155" s="14"/>
       <c r="V155" s="14"/>
     </row>
-    <row r="156" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" ht="14.45" customHeight="1">
       <c r="A156" s="14" t="s">
         <v>460</v>
       </c>
@@ -14285,7 +14305,7 @@
       <c r="U156" s="14"/>
       <c r="V156" s="14"/>
     </row>
-    <row r="157" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" ht="14.45" customHeight="1">
       <c r="A157" s="14" t="s">
         <v>460</v>
       </c>
@@ -14346,7 +14366,7 @@
       <c r="U157" s="14"/>
       <c r="V157" s="14"/>
     </row>
-    <row r="158" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" ht="14.45" customHeight="1">
       <c r="A158" s="14" t="s">
         <v>460</v>
       </c>
@@ -14407,7 +14427,7 @@
       <c r="U158" s="14"/>
       <c r="V158" s="14"/>
     </row>
-    <row r="159" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" ht="14.45" customHeight="1">
       <c r="A159" s="14" t="s">
         <v>460</v>
       </c>
@@ -14468,7 +14488,7 @@
       <c r="U159" s="14"/>
       <c r="V159" s="14"/>
     </row>
-    <row r="160" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" ht="14.45" customHeight="1">
       <c r="A160" s="14" t="s">
         <v>460</v>
       </c>
@@ -14529,7 +14549,7 @@
       <c r="U160" s="14"/>
       <c r="V160" s="14"/>
     </row>
-    <row r="161" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:22" ht="14.45" customHeight="1">
       <c r="A161" s="14" t="s">
         <v>460</v>
       </c>
@@ -14590,7 +14610,7 @@
       <c r="U161" s="14"/>
       <c r="V161" s="14"/>
     </row>
-    <row r="162" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:22" ht="14.45" customHeight="1">
       <c r="A162" s="14" t="s">
         <v>460</v>
       </c>
@@ -14651,7 +14671,7 @@
       <c r="U162" s="14"/>
       <c r="V162" s="14"/>
     </row>
-    <row r="163" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:22" ht="14.45" customHeight="1">
       <c r="A163" s="14" t="s">
         <v>460</v>
       </c>
@@ -14712,7 +14732,7 @@
       <c r="U163" s="14"/>
       <c r="V163" s="14"/>
     </row>
-    <row r="164" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:22" ht="14.45" customHeight="1">
       <c r="A164" s="14" t="s">
         <v>460</v>
       </c>
@@ -14773,7 +14793,7 @@
       <c r="U164" s="14"/>
       <c r="V164" s="14"/>
     </row>
-    <row r="165" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:22" ht="14.45" customHeight="1">
       <c r="A165" s="14" t="s">
         <v>460</v>
       </c>
@@ -14834,7 +14854,7 @@
       <c r="U165" s="14"/>
       <c r="V165" s="14"/>
     </row>
-    <row r="166" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:22" ht="14.45" customHeight="1">
       <c r="A166" s="14" t="s">
         <v>460</v>
       </c>
@@ -14895,7 +14915,7 @@
       <c r="U166" s="14"/>
       <c r="V166" s="14"/>
     </row>
-    <row r="167" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:22" ht="14.45" customHeight="1">
       <c r="A167" s="14" t="s">
         <v>460</v>
       </c>
@@ -14956,7 +14976,7 @@
       <c r="U167" s="14"/>
       <c r="V167" s="14"/>
     </row>
-    <row r="168" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:22" ht="14.45" customHeight="1">
       <c r="A168" s="14" t="s">
         <v>460</v>
       </c>
@@ -15015,7 +15035,7 @@
       <c r="U168" s="14"/>
       <c r="V168" s="14"/>
     </row>
-    <row r="169" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:22" ht="14.45" customHeight="1">
       <c r="A169" s="14" t="s">
         <v>460</v>
       </c>
@@ -15074,7 +15094,7 @@
       <c r="U169" s="14"/>
       <c r="V169" s="14"/>
     </row>
-    <row r="170" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:22" ht="14.45" customHeight="1">
       <c r="A170" s="14" t="s">
         <v>460</v>
       </c>
@@ -15133,7 +15153,7 @@
       <c r="U170" s="14"/>
       <c r="V170" s="14"/>
     </row>
-    <row r="171" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:22" ht="14.45" customHeight="1" thickBot="1">
       <c r="A171" s="14" t="s">
         <v>460</v>
       </c>
@@ -15192,7 +15212,7 @@
       <c r="U171" s="14"/>
       <c r="V171" s="14"/>
     </row>
-    <row r="172" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:22" ht="14.45" customHeight="1">
       <c r="A172" s="31" t="s">
         <v>27</v>
       </c>
@@ -15258,7 +15278,7 @@
       </c>
       <c r="V172" s="34"/>
     </row>
-    <row r="173" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:22" ht="14.45" customHeight="1">
       <c r="A173" s="35" t="s">
         <v>27</v>
       </c>
@@ -15322,7 +15342,7 @@
       <c r="U173" s="14"/>
       <c r="V173" s="36"/>
     </row>
-    <row r="174" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:22" ht="14.45" customHeight="1">
       <c r="A174" s="35" t="s">
         <v>27</v>
       </c>
@@ -15381,7 +15401,7 @@
       <c r="U174" s="14"/>
       <c r="V174" s="36"/>
     </row>
-    <row r="175" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:22" ht="14.45" customHeight="1">
       <c r="A175" s="35" t="s">
         <v>27</v>
       </c>
@@ -15447,7 +15467,7 @@
       <c r="U175" s="14"/>
       <c r="V175" s="36"/>
     </row>
-    <row r="176" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:22" ht="14.45" customHeight="1">
       <c r="A176" s="35" t="s">
         <v>27</v>
       </c>
@@ -15506,7 +15526,7 @@
       <c r="U176" s="14"/>
       <c r="V176" s="36"/>
     </row>
-    <row r="177" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:22" ht="14.45" customHeight="1">
       <c r="A177" s="35" t="s">
         <v>27</v>
       </c>
@@ -15571,7 +15591,7 @@
       <c r="U177" s="14"/>
       <c r="V177" s="36"/>
     </row>
-    <row r="178" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:22" ht="14.45" customHeight="1">
       <c r="A178" s="35" t="s">
         <v>27</v>
       </c>
@@ -15630,7 +15650,7 @@
       <c r="U178" s="14"/>
       <c r="V178" s="36"/>
     </row>
-    <row r="179" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:22" ht="14.45" customHeight="1">
       <c r="A179" s="35" t="s">
         <v>27</v>
       </c>
@@ -15689,7 +15709,7 @@
       <c r="U179" s="14"/>
       <c r="V179" s="36"/>
     </row>
-    <row r="180" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:22" ht="14.45" customHeight="1">
       <c r="A180" s="35" t="s">
         <v>27</v>
       </c>
@@ -15748,7 +15768,7 @@
       <c r="U180" s="14"/>
       <c r="V180" s="36"/>
     </row>
-    <row r="181" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:22" ht="14.45" customHeight="1">
       <c r="A181" s="35" t="s">
         <v>27</v>
       </c>
@@ -15807,7 +15827,7 @@
       <c r="U181" s="14"/>
       <c r="V181" s="36"/>
     </row>
-    <row r="182" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:22" ht="14.45" customHeight="1" thickBot="1">
       <c r="A182" s="37" t="s">
         <v>27</v>
       </c>
@@ -15866,7 +15886,7 @@
       <c r="U182" s="39"/>
       <c r="V182" s="40"/>
     </row>
-    <row r="183" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:22" ht="14.45" customHeight="1">
       <c r="A183" s="31" t="s">
         <v>27</v>
       </c>
@@ -15932,7 +15952,7 @@
       </c>
       <c r="V183" s="34"/>
     </row>
-    <row r="184" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:22" ht="14.45" customHeight="1">
       <c r="A184" s="35" t="s">
         <v>27</v>
       </c>
@@ -15996,7 +16016,7 @@
       <c r="U184" s="14"/>
       <c r="V184" s="36"/>
     </row>
-    <row r="185" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:22" ht="14.45" customHeight="1">
       <c r="A185" s="35" t="s">
         <v>27</v>
       </c>
@@ -16055,7 +16075,7 @@
       <c r="U185" s="14"/>
       <c r="V185" s="36"/>
     </row>
-    <row r="186" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:22" ht="14.45" customHeight="1">
       <c r="A186" s="35" t="s">
         <v>27</v>
       </c>
@@ -16117,7 +16137,7 @@
       <c r="U186" s="14"/>
       <c r="V186" s="36"/>
     </row>
-    <row r="187" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:22" ht="14.45" customHeight="1">
       <c r="A187" s="35" t="s">
         <v>27</v>
       </c>
@@ -16176,7 +16196,7 @@
       <c r="U187" s="14"/>
       <c r="V187" s="36"/>
     </row>
-    <row r="188" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:22" ht="14.45" customHeight="1">
       <c r="A188" s="35" t="s">
         <v>27</v>
       </c>
@@ -16235,7 +16255,7 @@
       <c r="U188" s="14"/>
       <c r="V188" s="36"/>
     </row>
-    <row r="189" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:22" ht="14.45" customHeight="1">
       <c r="A189" s="35" t="s">
         <v>27</v>
       </c>
@@ -16294,7 +16314,7 @@
       <c r="U189" s="14"/>
       <c r="V189" s="36"/>
     </row>
-    <row r="190" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:22" ht="14.45" customHeight="1">
       <c r="A190" s="35" t="s">
         <v>27</v>
       </c>
@@ -16353,7 +16373,7 @@
       <c r="U190" s="14"/>
       <c r="V190" s="36"/>
     </row>
-    <row r="191" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:22" ht="14.45" customHeight="1">
       <c r="A191" s="35" t="s">
         <v>27</v>
       </c>
@@ -16412,7 +16432,7 @@
       <c r="U191" s="14"/>
       <c r="V191" s="36"/>
     </row>
-    <row r="192" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:22" ht="14.45" customHeight="1">
       <c r="A192" s="35" t="s">
         <v>27</v>
       </c>
@@ -16471,7 +16491,7 @@
       <c r="U192" s="14"/>
       <c r="V192" s="36"/>
     </row>
-    <row r="193" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:22" ht="14.45" customHeight="1" thickBot="1">
       <c r="A193" s="37" t="s">
         <v>27</v>
       </c>
@@ -16530,7 +16550,7 @@
       <c r="U193" s="39"/>
       <c r="V193" s="40"/>
     </row>
-    <row r="194" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:22" ht="14.45" customHeight="1">
       <c r="A194" s="31" t="s">
         <v>27</v>
       </c>
@@ -16596,7 +16616,7 @@
       </c>
       <c r="V194" s="34"/>
     </row>
-    <row r="195" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:22" ht="14.45" customHeight="1">
       <c r="A195" s="35" t="s">
         <v>27</v>
       </c>
@@ -16660,7 +16680,7 @@
       <c r="U195" s="14"/>
       <c r="V195" s="36"/>
     </row>
-    <row r="196" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:22" ht="14.45" customHeight="1">
       <c r="A196" s="35" t="s">
         <v>27</v>
       </c>
@@ -16719,7 +16739,7 @@
       <c r="U196" s="14"/>
       <c r="V196" s="36"/>
     </row>
-    <row r="197" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:22" ht="14.45" customHeight="1">
       <c r="A197" s="35" t="s">
         <v>27</v>
       </c>
@@ -16785,7 +16805,7 @@
       <c r="U197" s="14"/>
       <c r="V197" s="36"/>
     </row>
-    <row r="198" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:22" ht="14.45" customHeight="1">
       <c r="A198" s="35" t="s">
         <v>27</v>
       </c>
@@ -16844,7 +16864,7 @@
       <c r="U198" s="14"/>
       <c r="V198" s="36"/>
     </row>
-    <row r="199" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:22" ht="14.45" customHeight="1">
       <c r="A199" s="35" t="s">
         <v>27</v>
       </c>
@@ -16909,7 +16929,7 @@
       <c r="U199" s="14"/>
       <c r="V199" s="36"/>
     </row>
-    <row r="200" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:22" ht="14.45" customHeight="1">
       <c r="A200" s="35" t="s">
         <v>27</v>
       </c>
@@ -16968,7 +16988,7 @@
       <c r="U200" s="14"/>
       <c r="V200" s="36"/>
     </row>
-    <row r="201" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:22" ht="14.45" customHeight="1">
       <c r="A201" s="35" t="s">
         <v>27</v>
       </c>
@@ -17027,7 +17047,7 @@
       <c r="U201" s="14"/>
       <c r="V201" s="36"/>
     </row>
-    <row r="202" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:22" ht="14.45" customHeight="1">
       <c r="A202" s="35" t="s">
         <v>27</v>
       </c>
@@ -17086,7 +17106,7 @@
       <c r="U202" s="14"/>
       <c r="V202" s="36"/>
     </row>
-    <row r="203" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:22" ht="14.45" customHeight="1">
       <c r="A203" s="35" t="s">
         <v>27</v>
       </c>
@@ -17145,7 +17165,7 @@
       <c r="U203" s="14"/>
       <c r="V203" s="36"/>
     </row>
-    <row r="204" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:22" ht="14.45" customHeight="1" thickBot="1">
       <c r="A204" s="37" t="s">
         <v>27</v>
       </c>
@@ -17204,7 +17224,7 @@
       <c r="U204" s="39"/>
       <c r="V204" s="40"/>
     </row>
-    <row r="205" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:22" ht="14.45" customHeight="1">
       <c r="A205" s="31" t="s">
         <v>27</v>
       </c>
@@ -17270,7 +17290,7 @@
       </c>
       <c r="V205" s="34"/>
     </row>
-    <row r="206" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:22" ht="14.45" customHeight="1">
       <c r="A206" s="35" t="s">
         <v>27</v>
       </c>
@@ -17334,7 +17354,7 @@
       <c r="U206" s="14"/>
       <c r="V206" s="36"/>
     </row>
-    <row r="207" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:22" ht="14.45" customHeight="1">
       <c r="A207" s="35" t="s">
         <v>27</v>
       </c>
@@ -17393,7 +17413,7 @@
       <c r="U207" s="14"/>
       <c r="V207" s="36"/>
     </row>
-    <row r="208" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:22" ht="14.45" customHeight="1">
       <c r="A208" s="35" t="s">
         <v>27</v>
       </c>
@@ -17459,7 +17479,7 @@
       <c r="U208" s="14"/>
       <c r="V208" s="36"/>
     </row>
-    <row r="209" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:22" ht="14.45" customHeight="1">
       <c r="A209" s="35" t="s">
         <v>27</v>
       </c>
@@ -17518,7 +17538,7 @@
       <c r="U209" s="14"/>
       <c r="V209" s="36"/>
     </row>
-    <row r="210" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:22" ht="14.45" customHeight="1">
       <c r="A210" s="35" t="s">
         <v>27</v>
       </c>
@@ -17577,7 +17597,7 @@
       <c r="U210" s="14"/>
       <c r="V210" s="36"/>
     </row>
-    <row r="211" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:22" ht="14.45" customHeight="1">
       <c r="A211" s="35" t="s">
         <v>27</v>
       </c>
@@ -17636,7 +17656,7 @@
       <c r="U211" s="14"/>
       <c r="V211" s="36"/>
     </row>
-    <row r="212" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:22" ht="14.45" customHeight="1">
       <c r="A212" s="35" t="s">
         <v>27</v>
       </c>
@@ -17695,7 +17715,7 @@
       <c r="U212" s="14"/>
       <c r="V212" s="36"/>
     </row>
-    <row r="213" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:22" ht="14.45" customHeight="1">
       <c r="A213" s="35" t="s">
         <v>27</v>
       </c>
@@ -17754,7 +17774,7 @@
       <c r="U213" s="14"/>
       <c r="V213" s="36"/>
     </row>
-    <row r="214" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:22" ht="14.45" customHeight="1">
       <c r="A214" s="35" t="s">
         <v>27</v>
       </c>
@@ -17813,7 +17833,7 @@
       <c r="U214" s="14"/>
       <c r="V214" s="36"/>
     </row>
-    <row r="215" spans="1:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:22" ht="14.45" customHeight="1" thickBot="1">
       <c r="A215" s="37" t="s">
         <v>27</v>
       </c>
@@ -17883,13 +17903,13 @@
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="F1">
-    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17897,12 +17917,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="aca03388-b78c-4415-a826-d0bf4eb594c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MigrationWizIdPermissions xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
+    <MigrationWizId xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
+    <MigrationWizIdVersion xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f0 xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18125,33 +18151,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="aca03388-b78c-4415-a826-d0bf4eb594c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MigrationWizIdPermissions xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
-    <MigrationWizId xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
-    <MigrationWizIdVersion xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f0 xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8016C37-55EC-4E22-8DA4-5D0423CAAC3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDD06CB-A440-48B1-8DB6-CCAE7949D7BC}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC5C007E-8165-41BE-9A06-7E3FC76D2AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -18166,4 +18174,31 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDD06CB-A440-48B1-8DB6-CCAE7949D7BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="383b0bb7-e620-4e20-ae9e-4f262a20ab07"/>
+    <ds:schemaRef ds:uri="aca03388-b78c-4415-a826-d0bf4eb594c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8016C37-55EC-4E22-8DA4-5D0423CAAC3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>